<commit_message>
updated bau gauranteed dispatch
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\RMI_all_states\RI\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57C83C38-8865-4F3F-B76A-27B1CF79E1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFB69B6C-7976-45F5-B632-0A00ED622DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="12735" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11460" yWindow="1320" windowWidth="17310" windowHeight="16080" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -521,18 +521,18 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -888,28 +888,28 @@
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="4">
-        <v>44854</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="C1" s="2">
+        <v>44855</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="str">
+      <c r="B2" s="4" t="str">
         <f>LOOKUP(B1,I1:J50,J1:J50)</f>
         <v>RI</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -917,10 +917,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -928,10 +928,10 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -939,10 +939,10 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -950,18 +950,18 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -969,10 +969,10 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -980,10 +980,10 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -991,10 +991,10 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1002,322 +1002,322 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="35" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J36" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="37" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J40" s="5" t="s">
+      <c r="J40" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="J41" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="42" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J43" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="46" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J46" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I47" s="5" t="s">
+      <c r="I47" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J47" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I48" s="5" t="s">
+      <c r="I48" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="J48" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="49" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I50" s="5" t="s">
+      <c r="I50" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J50" s="5" t="s">
+      <c r="J50" s="3" t="s">
         <v>77</v>
       </c>
     </row>
@@ -87074,10 +87074,10 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="6"/>
       <c r="D3" t="s">
         <v>135</v>
       </c>
@@ -87086,11 +87086,11 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <f>SUMIFS('all_csv_BECF-pre-ret'!D:D,'all_csv_BECF-pre-ret'!B:B,B4,'all_csv_BECF-pre-ret'!AI:AI,calcs!$C$1)</f>
         <v>0.02</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <f>C4/PTCF!B2</f>
         <v>2.2222222222222223E-2</v>
       </c>
@@ -87099,11 +87099,11 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <f>SUMIFS('all_csv_BECF-pre-ret'!D:D,'all_csv_BECF-pre-ret'!B:B,B5,'all_csv_BECF-pre-ret'!AI:AI,calcs!$C$1)</f>
         <v>0.51532905399999995</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <f>C5/PTCF!B3</f>
         <v>0.57258783777777766</v>
       </c>
@@ -87112,11 +87112,11 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <f>SUMIFS('all_csv_BECF-pre-ret'!D:D,'all_csv_BECF-pre-ret'!B:B,B6,'all_csv_BECF-pre-ret'!AI:AI,calcs!$C$1)</f>
         <v>0.02</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <f>C6/PTCF!B12</f>
         <v>2.2222222222222223E-2</v>
       </c>
@@ -87336,7 +87336,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -87346,10 +87346,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="9">
         <v>2015</v>
       </c>
       <c r="C1">
@@ -87759,147 +87759,147 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -87907,147 +87907,147 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -88055,147 +88055,147 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -88203,147 +88203,147 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -88351,147 +88351,147 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -88499,147 +88499,147 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK14" si="2">$B9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -88647,147 +88647,147 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -88962,8 +88962,8 @@
         <v>0</v>
       </c>
       <c r="G12" s="10">
-        <f>calcs!D5</f>
-        <v>0.57258783777777766</v>
+        <f>calcs!D6</f>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
@@ -89239,147 +89239,147 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -89613,147 +89613,147 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <f>B17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:AK17" si="3">C17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>